<commit_message>
Added GLORIA root region definitions
</commit_message>
<xml_diff>
--- a/concs/RootRegionLegend.xlsx
+++ b/concs/RootRegionLegend.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobfry/Desktop/Projects/isa_projects/IELab/local/Roots/GlobalIELab/Settings/Root/Legends/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobfry/repos/make-labour-satellite/concs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FB113E-D9B4-8242-8395-C4041B07616B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30887C9-F14E-224D-A7C7-FFA866F227EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27940" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="README" sheetId="5" r:id="rId1"/>
-    <sheet name="RootCountryLegend" sheetId="1" r:id="rId2"/>
+    <sheet name="RootCountryLegend" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3560" uniqueCount="1014">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3554" uniqueCount="1008">
   <si>
     <t>Root country number</t>
   </si>
@@ -2938,9 +2937,6 @@
     <t>Slovak Republic</t>
   </si>
   <si>
-    <t>Some tools for querying this file can be found in: /import/emily1/isa/Programs/Tools/root_country_legend</t>
-  </si>
-  <si>
     <t>FAO</t>
   </si>
   <si>
@@ -2984,21 +2980,6 @@
   </si>
   <si>
     <t>DRE</t>
-  </si>
-  <si>
-    <t>In sheet RootCountryLegend please do not add any columns before existing columns. Add new columns to the end.</t>
-  </si>
-  <si>
-    <t>In sheet RootCountryLegend, do not include empty cells, use the placeholder 'ZZZZ' instead.</t>
-  </si>
-  <si>
-    <t>If new name columns are added, check root country toolbox functions as new column may need to be added to search scope</t>
-  </si>
-  <si>
-    <t>After updating this file, run test_runner.m in the the toolbox to ensure your changes have not broken existing functionality.</t>
-  </si>
-  <si>
-    <t>Instructions:</t>
   </si>
   <si>
     <t>RE</t>
@@ -3421,56 +3402,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A7"/>
-  <sheetViews>
-    <sheetView showRuler="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>986</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>984</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R222"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L181" sqref="L181"/>
     </sheetView>
   </sheetViews>
@@ -3523,22 +3459,22 @@
         <v>936</v>
       </c>
       <c r="M1" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="N1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="O1" t="s">
-        <v>993</v>
+        <v>987</v>
       </c>
       <c r="P1" t="s">
-        <v>1002</v>
+        <v>996</v>
       </c>
       <c r="Q1" t="s">
+        <v>998</v>
+      </c>
+      <c r="R1" t="s">
         <v>1004</v>
-      </c>
-      <c r="R1" t="s">
-        <v>1010</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -3921,7 +3857,7 @@
         <v>9</v>
       </c>
       <c r="O8" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="P8" t="s">
         <v>9</v>
@@ -5371,7 +5307,7 @@
         <v>140</v>
       </c>
       <c r="M34" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="N34" t="s">
         <v>9</v>
@@ -5595,16 +5531,16 @@
         <v>156</v>
       </c>
       <c r="M38" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>1012</v>
+        <v>1006</v>
       </c>
       <c r="O38" t="s">
         <v>9</v>
       </c>
       <c r="P38" t="s">
-        <v>1003</v>
+        <v>997</v>
       </c>
       <c r="Q38" t="s">
         <v>9</v>
@@ -5651,13 +5587,13 @@
         <v>384</v>
       </c>
       <c r="M39" t="s">
-        <v>992</v>
+        <v>986</v>
       </c>
       <c r="N39" t="s">
         <v>9</v>
       </c>
       <c r="O39" t="s">
-        <v>995</v>
+        <v>989</v>
       </c>
       <c r="P39" t="s">
         <v>9</v>
@@ -5763,7 +5699,7 @@
         <v>180</v>
       </c>
       <c r="M41" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="N41" t="s">
         <v>9</v>
@@ -6435,7 +6371,7 @@
         <v>203</v>
       </c>
       <c r="M53" t="s">
-        <v>991</v>
+        <v>985</v>
       </c>
       <c r="N53" t="s">
         <v>9</v>
@@ -6739,28 +6675,28 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>980</v>
+      </c>
+      <c r="C59" t="s">
+        <v>980</v>
+      </c>
+      <c r="D59" t="s">
         <v>981</v>
       </c>
-      <c r="C59" t="s">
-        <v>981</v>
-      </c>
-      <c r="D59" t="s">
-        <v>987</v>
-      </c>
       <c r="E59" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="F59" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="G59" t="s">
-        <v>988</v>
+        <v>982</v>
       </c>
       <c r="H59" t="s">
-        <v>989</v>
+        <v>983</v>
       </c>
       <c r="I59" t="s">
-        <v>990</v>
+        <v>984</v>
       </c>
       <c r="J59" t="s">
         <v>918</v>
@@ -6778,7 +6714,7 @@
         <v>9</v>
       </c>
       <c r="O59" t="s">
-        <v>996</v>
+        <v>990</v>
       </c>
       <c r="P59" t="s">
         <v>9</v>
@@ -7231,7 +7167,7 @@
         <v>9</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>996</v>
+        <v>990</v>
       </c>
       <c r="O67" t="s">
         <v>9</v>
@@ -7345,7 +7281,7 @@
         <v>9</v>
       </c>
       <c r="N69" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="O69" t="s">
         <v>9</v>
@@ -8257,10 +8193,10 @@
         <v>9</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>994</v>
+        <v>988</v>
       </c>
       <c r="O85" t="s">
-        <v>994</v>
+        <v>988</v>
       </c>
       <c r="P85" t="s">
         <v>9</v>
@@ -9508,7 +9444,7 @@
         <v>410</v>
       </c>
       <c r="M107" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="N107" t="s">
         <v>9</v>
@@ -10291,7 +10227,7 @@
         <v>9</v>
       </c>
       <c r="H121" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I121" t="s">
         <v>506</v>
@@ -10312,13 +10248,13 @@
         <v>9</v>
       </c>
       <c r="O121" t="s">
+        <v>994</v>
+      </c>
+      <c r="P121" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q121" t="s">
         <v>1000</v>
-      </c>
-      <c r="P121" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q121" t="s">
-        <v>1006</v>
       </c>
       <c r="R121" t="s">
         <v>9</v>
@@ -10489,7 +10425,7 @@
         <v>9</v>
       </c>
       <c r="Q124" t="s">
-        <v>1008</v>
+        <v>1002</v>
       </c>
       <c r="R124" t="s">
         <v>9</v>
@@ -10762,22 +10698,22 @@
         <v>807</v>
       </c>
       <c r="M129" s="1" t="s">
-        <v>1011</v>
+        <v>1005</v>
       </c>
       <c r="N129" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="O129" s="1" t="s">
-        <v>1011</v>
+        <v>1005</v>
       </c>
       <c r="P129" t="s">
         <v>9</v>
       </c>
       <c r="Q129" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
       <c r="R129" t="s">
-        <v>1011</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.2">
@@ -12529,7 +12465,7 @@
         <v>408</v>
       </c>
       <c r="M160" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="N160" t="s">
         <v>9</v>
@@ -12700,7 +12636,7 @@
         <v>275</v>
       </c>
       <c r="M163" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="N163" t="s">
         <v>9</v>
@@ -13615,10 +13551,10 @@
         <v>9</v>
       </c>
       <c r="N179" s="1" t="s">
-        <v>1013</v>
+        <v>1007</v>
       </c>
       <c r="O179" s="1" t="s">
-        <v>1013</v>
+        <v>1007</v>
       </c>
       <c r="P179" t="s">
         <v>9</v>
@@ -13729,10 +13665,10 @@
         <v>9</v>
       </c>
       <c r="N181" s="1" t="s">
-        <v>998</v>
+        <v>992</v>
       </c>
       <c r="O181" t="s">
-        <v>998</v>
+        <v>992</v>
       </c>
       <c r="P181" t="s">
         <v>9</v>
@@ -14023,7 +13959,7 @@
         <v>9</v>
       </c>
       <c r="Q186" t="s">
-        <v>1009</v>
+        <v>1003</v>
       </c>
       <c r="R186" t="s">
         <v>9</v>
@@ -14053,7 +13989,7 @@
         <v>9</v>
       </c>
       <c r="H187" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I187" t="s">
         <v>9</v>
@@ -14593,7 +14529,7 @@
         <v>9</v>
       </c>
       <c r="Q196" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="R196" t="s">
         <v>9</v>
@@ -14929,7 +14865,7 @@
         <v>9</v>
       </c>
       <c r="O202" t="s">
-        <v>1001</v>
+        <v>995</v>
       </c>
       <c r="P202" t="s">
         <v>9</v>
@@ -15550,7 +15486,7 @@
         <v>92</v>
       </c>
       <c r="M213" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="N213" t="s">
         <v>9</v>
@@ -15607,7 +15543,7 @@
         <v>704</v>
       </c>
       <c r="M214" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="N214" t="s">
         <v>9</v>
@@ -15898,7 +15834,7 @@
         <v>9</v>
       </c>
       <c r="O219" t="s">
-        <v>999</v>
+        <v>993</v>
       </c>
       <c r="P219" t="s">
         <v>9</v>

</xml_diff>